<commit_message>
notes revisions and rubric changed to 40 max
</commit_message>
<xml_diff>
--- a/LabStarters/Lab01/Lab01Rubric_CS195.xlsx
+++ b/LabStarters/Lab01/Lab01Rubric_CS195.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2395E803-C8AE-1C4E-B170-2F4283409503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A4334F9-C307-4D1E-8EC2-744226AF76D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7580" yWindow="500" windowWidth="12620" windowHeight="14660" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="5748" yWindow="1284" windowWidth="22944" windowHeight="11592" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -145,20 +156,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,25 +488,22 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.19921875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -505,115 +512,110 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f>SUM(B4:B11)</f>
-        <v>50</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -628,40 +630,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.69921875" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" customWidth="1"/>
+    <col min="3" max="3" width="6.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,141 +674,135 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <f>SUM(B7:B14)</f>
-        <v>50</v>
-      </c>
-      <c r="C17" s="5">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4">
         <f>SUM(C7:C14)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
   </sheetData>
@@ -814,5 +810,6 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>